<commit_message>
fix response to no configuration file
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hterauchi\Desktop\mondayApp\MondayBoardUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07599CD0-B8C3-4430-ACCC-ED927A90335A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E70CFF-A8F8-43F0-ADFD-C9A2BA0DBFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A014528C-4C02-414A-8924-1BB9672EFFE2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Request Type</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Yoshi Ilands 2</t>
+  </si>
+  <si>
+    <t>Email design for summer dinner</t>
   </si>
 </sst>
 </file>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB12E390-2C9C-4CAB-9E07-C95BABA9EA26}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +622,46 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44051</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43657</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>